<commit_message>
chore: update beta example dict
</commit_message>
<xml_diff>
--- a/dictionaries/example-dictionary/example_dictionary.xlsx
+++ b/dictionaries/example-dictionary/example_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/example-dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ED25FB52-9E0E-BE44-AB84-F4A19C4401E2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784A9E17-123C-F741-BECA-530314291C46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12600" yWindow="460" windowWidth="15960" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
-  <si>
-    <t>table</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -32,72 +29,84 @@
     <t>valueType</t>
   </si>
   <si>
-    <t>entityType</t>
-  </si>
-  <si>
-    <t>referencedEntityType</t>
-  </si>
-  <si>
-    <t>mimeType</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
-    <t>repeatable</t>
-  </si>
-  <si>
-    <t>occurrenceGroup</t>
-  </si>
-  <si>
-    <t>index</t>
-  </si>
-  <si>
     <t>age</t>
   </si>
   <si>
     <t>Integer</t>
   </si>
   <si>
-    <t>Patient</t>
-  </si>
-  <si>
-    <t>Numeric</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
     <t>variable</t>
   </si>
   <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>missing</t>
-  </si>
-  <si>
-    <t>tutorial_beginner</t>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Age of the child</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>Name of the child</t>
+  </si>
+  <si>
+    <t>child_id</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>Unique identifier of the child_id</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Country of the child</t>
+  </si>
+  <si>
+    <t>isMissing</t>
+  </si>
+  <si>
+    <t>gb</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>ne</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Great Brittain</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>ge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,14 +144,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1315,19 +1322,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IV10"/>
+  <dimension ref="A1:IP5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="256" width="8.83203125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="8.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="250" width="8.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1338,160 +1346,308 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="4"/>
+      <c r="AT2" s="4"/>
+      <c r="AU2" s="4"/>
+      <c r="AV2" s="4"/>
+      <c r="AW2" s="4"/>
+      <c r="AX2" s="4"/>
+      <c r="AY2" s="4"/>
+      <c r="AZ2" s="4"/>
+      <c r="BA2" s="4"/>
+      <c r="BB2" s="4"/>
+      <c r="BC2" s="4"/>
+      <c r="BD2" s="4"/>
+      <c r="BE2" s="4"/>
+      <c r="BF2" s="4"/>
+      <c r="BG2" s="4"/>
+      <c r="BH2" s="4"/>
+      <c r="BI2" s="4"/>
+      <c r="BJ2" s="4"/>
+      <c r="BK2" s="4"/>
+      <c r="BL2" s="4"/>
+      <c r="BM2" s="4"/>
+      <c r="BN2" s="4"/>
+      <c r="BO2" s="4"/>
+      <c r="BP2" s="4"/>
+      <c r="BQ2" s="4"/>
+      <c r="BR2" s="4"/>
+      <c r="BS2" s="4"/>
+      <c r="BT2" s="4"/>
+      <c r="BU2" s="4"/>
+      <c r="BV2" s="4"/>
+      <c r="BW2" s="4"/>
+      <c r="BX2" s="4"/>
+      <c r="BY2" s="4"/>
+      <c r="BZ2" s="4"/>
+      <c r="CA2" s="4"/>
+      <c r="CB2" s="4"/>
+      <c r="CC2" s="4"/>
+      <c r="CD2" s="4"/>
+      <c r="CE2" s="4"/>
+      <c r="CF2" s="4"/>
+      <c r="CG2" s="4"/>
+      <c r="CH2" s="4"/>
+      <c r="CI2" s="4"/>
+      <c r="CJ2" s="4"/>
+      <c r="CK2" s="4"/>
+      <c r="CL2" s="4"/>
+      <c r="CM2" s="4"/>
+      <c r="CN2" s="4"/>
+      <c r="CO2" s="4"/>
+      <c r="CP2" s="4"/>
+      <c r="CQ2" s="4"/>
+      <c r="CR2" s="4"/>
+      <c r="CS2" s="4"/>
+      <c r="CT2" s="4"/>
+      <c r="CU2" s="4"/>
+      <c r="CV2" s="4"/>
+      <c r="CW2" s="4"/>
+      <c r="CX2" s="4"/>
+      <c r="CY2" s="4"/>
+      <c r="CZ2" s="4"/>
+      <c r="DA2" s="4"/>
+      <c r="DB2" s="4"/>
+      <c r="DC2" s="4"/>
+      <c r="DD2" s="4"/>
+      <c r="DE2" s="4"/>
+      <c r="DF2" s="4"/>
+      <c r="DG2" s="4"/>
+      <c r="DH2" s="4"/>
+      <c r="DI2" s="4"/>
+      <c r="DJ2" s="4"/>
+      <c r="DK2" s="4"/>
+      <c r="DL2" s="4"/>
+      <c r="DM2" s="4"/>
+      <c r="DN2" s="4"/>
+      <c r="DO2" s="4"/>
+      <c r="DP2" s="4"/>
+      <c r="DQ2" s="4"/>
+      <c r="DR2" s="4"/>
+      <c r="DS2" s="4"/>
+      <c r="DT2" s="4"/>
+      <c r="DU2" s="4"/>
+      <c r="DV2" s="4"/>
+      <c r="DW2" s="4"/>
+      <c r="DX2" s="4"/>
+      <c r="DY2" s="4"/>
+      <c r="DZ2" s="4"/>
+      <c r="EA2" s="4"/>
+      <c r="EB2" s="4"/>
+      <c r="EC2" s="4"/>
+      <c r="ED2" s="4"/>
+      <c r="EE2" s="4"/>
+      <c r="EF2" s="4"/>
+      <c r="EG2" s="4"/>
+      <c r="EH2" s="4"/>
+      <c r="EI2" s="4"/>
+      <c r="EJ2" s="4"/>
+      <c r="EK2" s="4"/>
+      <c r="EL2" s="4"/>
+      <c r="EM2" s="4"/>
+      <c r="EN2" s="4"/>
+      <c r="EO2" s="4"/>
+      <c r="EP2" s="4"/>
+      <c r="EQ2" s="4"/>
+      <c r="ER2" s="4"/>
+      <c r="ES2" s="4"/>
+      <c r="ET2" s="4"/>
+      <c r="EU2" s="4"/>
+      <c r="EV2" s="4"/>
+      <c r="EW2" s="4"/>
+      <c r="EX2" s="4"/>
+      <c r="EY2" s="4"/>
+      <c r="EZ2" s="4"/>
+      <c r="FA2" s="4"/>
+      <c r="FB2" s="4"/>
+      <c r="FC2" s="4"/>
+      <c r="FD2" s="4"/>
+      <c r="FE2" s="4"/>
+      <c r="FF2" s="4"/>
+      <c r="FG2" s="4"/>
+      <c r="FH2" s="4"/>
+      <c r="FI2" s="4"/>
+      <c r="FJ2" s="4"/>
+      <c r="FK2" s="4"/>
+      <c r="FL2" s="4"/>
+      <c r="FM2" s="4"/>
+      <c r="FN2" s="4"/>
+      <c r="FO2" s="4"/>
+      <c r="FP2" s="4"/>
+      <c r="FQ2" s="4"/>
+      <c r="FR2" s="4"/>
+      <c r="FS2" s="4"/>
+      <c r="FT2" s="4"/>
+      <c r="FU2" s="4"/>
+      <c r="FV2" s="4"/>
+      <c r="FW2" s="4"/>
+      <c r="FX2" s="4"/>
+      <c r="FY2" s="4"/>
+      <c r="FZ2" s="4"/>
+      <c r="GA2" s="4"/>
+      <c r="GB2" s="4"/>
+      <c r="GC2" s="4"/>
+      <c r="GD2" s="4"/>
+      <c r="GE2" s="4"/>
+      <c r="GF2" s="4"/>
+      <c r="GG2" s="4"/>
+      <c r="GH2" s="4"/>
+      <c r="GI2" s="4"/>
+      <c r="GJ2" s="4"/>
+      <c r="GK2" s="4"/>
+      <c r="GL2" s="4"/>
+      <c r="GM2" s="4"/>
+      <c r="GN2" s="4"/>
+      <c r="GO2" s="4"/>
+      <c r="GP2" s="4"/>
+      <c r="GQ2" s="4"/>
+      <c r="GR2" s="4"/>
+      <c r="GS2" s="4"/>
+      <c r="GT2" s="4"/>
+      <c r="GU2" s="4"/>
+      <c r="GV2" s="4"/>
+      <c r="GW2" s="4"/>
+      <c r="GX2" s="4"/>
+      <c r="GY2" s="4"/>
+      <c r="GZ2" s="4"/>
+      <c r="HA2" s="4"/>
+      <c r="HB2" s="4"/>
+      <c r="HC2" s="4"/>
+      <c r="HD2" s="4"/>
+      <c r="HE2" s="4"/>
+      <c r="HF2" s="4"/>
+      <c r="HG2" s="4"/>
+      <c r="HH2" s="4"/>
+      <c r="HI2" s="4"/>
+      <c r="HJ2" s="4"/>
+      <c r="HK2" s="4"/>
+      <c r="HL2" s="4"/>
+      <c r="HM2" s="4"/>
+      <c r="HN2" s="4"/>
+      <c r="HO2" s="4"/>
+      <c r="HP2" s="4"/>
+      <c r="HQ2" s="4"/>
+      <c r="HR2" s="4"/>
+      <c r="HS2" s="4"/>
+      <c r="HT2" s="4"/>
+      <c r="HU2" s="4"/>
+      <c r="HV2" s="4"/>
+      <c r="HW2" s="4"/>
+      <c r="HX2" s="4"/>
+      <c r="HY2" s="4"/>
+      <c r="HZ2" s="4"/>
+      <c r="IA2" s="4"/>
+      <c r="IB2" s="4"/>
+      <c r="IC2" s="4"/>
+      <c r="ID2" s="4"/>
+      <c r="IE2" s="4"/>
+      <c r="IF2" s="4"/>
+      <c r="IG2" s="4"/>
+      <c r="IH2" s="4"/>
+      <c r="II2" s="4"/>
+      <c r="IJ2" s="4"/>
+      <c r="IK2" s="4"/>
+      <c r="IL2" s="4"/>
+      <c r="IM2" s="4"/>
+      <c r="IN2" s="4"/>
+      <c r="IO2" s="4"/>
+      <c r="IP2" s="4"/>
+    </row>
+    <row r="3" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1504,94 +1660,88 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:IV10"/>
+  <dimension ref="A1:IU5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="8.83203125" style="5" customWidth="1"/>
+    <col min="1" max="3" width="8.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="255" width="8.83203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="C3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="C5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: added fake data for beta dicts
</commit_message>
<xml_diff>
--- a/dictionaries/example-dictionary/example_dictionary.xlsx
+++ b/dictionaries/example-dictionary/example_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/example-dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784A9E17-123C-F741-BECA-530314291C46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DB511E-DA16-BE40-9C4F-440C375465A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="460" windowWidth="15960" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12600" yWindow="460" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Integer</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>variable</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
   </si>
   <si>
     <t>numeric</t>
-  </si>
-  <si>
-    <t>Name of the child</t>
   </si>
   <si>
     <t>child_id</t>
@@ -1322,10 +1316,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IP5"/>
+  <dimension ref="A1:IP4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1346,21 +1340,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1617,36 +1611,24 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="2" t="s">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1662,7 +1644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IU5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1675,72 +1657,72 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>